<commit_message>
cracion de hojas (estudiante, curso, notas)
</commit_message>
<xml_diff>
--- a/excel/16-ejecicio-excel-modificado.xlsx
+++ b/excel/16-ejecicio-excel-modificado.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCarvajal\Desktop\practicas\proyectos_pratica\evaluacion_cadean_tic\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC57AE8-1F4F-449F-856C-B33F1E70A8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1397A4A-5F97-4AB5-BC94-1CA5B785816D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="pagina1" sheetId="2" r:id="rId1"/>
-    <sheet name="pagina2" sheetId="1" r:id="rId2"/>
+    <sheet name="Estudiante" sheetId="2" r:id="rId1"/>
+    <sheet name="Curso" sheetId="1" r:id="rId2"/>
+    <sheet name="Nota" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -363,7 +364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -375,4 +376,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10175951-D2AB-423B-BD82-DC6B98F45C9C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
promedio, simbolo, manejo de caracter, encabezado y diseño de impresion, filtros
</commit_message>
<xml_diff>
--- a/excel/16-ejecicio-excel-modificado.xlsx
+++ b/excel/16-ejecicio-excel-modificado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCarvajal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCarvajal\Desktop\practicas\proyectos_pratica\evaluacion_cadean_tic\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1598922-5469-4F54-9DEF-93B06DE391D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4121A884-D039-4549-BD53-0F2F162AD8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,30 @@
     <sheet name="Curso" sheetId="2" r:id="rId2"/>
     <sheet name="Nota" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Curso!$A$1:$B$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Estudiante!$A$1:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Nota!$A$1:$H$11</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Código Estudiante</t>
   </si>
@@ -36,54 +54,54 @@
     <t>Jesús</t>
   </si>
   <si>
+    <t>'3116786765</t>
+  </si>
+  <si>
     <t>Alberto</t>
   </si>
   <si>
     <t>José</t>
   </si>
   <si>
+    <t>'3116986765</t>
+  </si>
+  <si>
     <t>María</t>
   </si>
   <si>
     <t>Sofía</t>
   </si>
   <si>
+    <t>'3121234567</t>
+  </si>
+  <si>
     <t>Carlos</t>
   </si>
   <si>
+    <t>'3132345678</t>
+  </si>
+  <si>
     <t>Laura</t>
   </si>
   <si>
+    <t>'3143456789</t>
+  </si>
+  <si>
     <t>Andrés</t>
   </si>
   <si>
+    <t>'3154567890</t>
+  </si>
+  <si>
     <t>Tatiana</t>
   </si>
   <si>
+    <t>'3165678901</t>
+  </si>
+  <si>
     <t>Felipe</t>
   </si>
   <si>
-    <t>'3116786765</t>
-  </si>
-  <si>
-    <t>'3116986765</t>
-  </si>
-  <si>
-    <t>'3121234567</t>
-  </si>
-  <si>
-    <t>'3132345678</t>
-  </si>
-  <si>
-    <t>'3143456789</t>
-  </si>
-  <si>
-    <t>'3154567890</t>
-  </si>
-  <si>
-    <t>'3165678901</t>
-  </si>
-  <si>
     <t>'3176789012</t>
   </si>
   <si>
@@ -118,6 +136,9 @@
   </si>
   <si>
     <t>Nota 3</t>
+  </si>
+  <si>
+    <t>Promedio</t>
   </si>
   <si>
     <t>3116786765</t>
@@ -144,7 +165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -191,13 +218,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,17 +531,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -534,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -542,10 +574,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -553,10 +585,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -564,10 +596,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -575,10 +607,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -586,10 +618,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -597,10 +629,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -608,10 +640,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -619,10 +651,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -630,23 +662,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <headerFooter>
+    <oddHeader>&amp;CRegistro Académico</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,29 +744,37 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <headerFooter>
+    <oddHeader>&amp;CRegistro Académico</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H11"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -751,8 +799,11 @@
       <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -763,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
@@ -777,8 +828,12 @@
       <c r="H2" s="2">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="5">
+        <f>AVERAGE($F2:$H2)</f>
+        <v>2.7666666666666671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -786,10 +841,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>23</v>
@@ -803,8 +858,12 @@
       <c r="H3" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="5">
+        <f>AVERAGE($F3:$H3)</f>
+        <v>3.2666666666666671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -812,10 +871,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>23</v>
@@ -829,8 +888,12 @@
       <c r="H4" s="2">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="5">
+        <f t="shared" ref="I4:I11" si="0">AVERAGE($F4:$H4)</f>
+        <v>3.3666666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -838,10 +901,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>23</v>
@@ -855,8 +918,12 @@
       <c r="H5" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5">
+        <f t="shared" si="0"/>
+        <v>3.4666666666666668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -864,10 +931,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -881,8 +948,12 @@
       <c r="H6" s="2">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="5">
+        <f t="shared" si="0"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -890,10 +961,10 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>23</v>
@@ -907,8 +978,12 @@
       <c r="H7" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -916,10 +991,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>23</v>
@@ -933,8 +1008,12 @@
       <c r="H8" s="2">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="5">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -942,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>23</v>
@@ -959,8 +1038,12 @@
       <c r="H9" s="2">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="5">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -968,10 +1051,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
@@ -985,8 +1068,12 @@
       <c r="H10" s="2">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="5">
+        <f t="shared" si="0"/>
+        <v>3.0333333333333332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -994,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>20</v>
@@ -1011,8 +1098,17 @@
       <c r="H11" s="2">
         <v>3.4</v>
       </c>
+      <c r="I11" s="5">
+        <f t="shared" si="0"/>
+        <v>3.1333333333333333</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H11" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape"/>
+  <headerFooter>
+    <oddHeader>&amp;CRegistro Académico</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ordamiento tabla (onombre estudiante y promedio), contar numero de participantes, calculo de curso, calculo de minimo y maximo
</commit_message>
<xml_diff>
--- a/excel/16-ejecicio-excel-modificado.xlsx
+++ b/excel/16-ejecicio-excel-modificado.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCarvajal\Desktop\practicas\proyectos_pratica\evaluacion_cadean_tic\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCarvajal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4121A884-D039-4549-BD53-0F2F162AD8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C695B7-DE76-4ACD-B045-C051270B934D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>Código Estudiante</t>
   </si>
@@ -142,6 +142,21 @@
   </si>
   <si>
     <t>3116786765</t>
+  </si>
+  <si>
+    <t>Resumen</t>
+  </si>
+  <si>
+    <t>Número de participantes</t>
+  </si>
+  <si>
+    <t>Promedio del curso</t>
+  </si>
+  <si>
+    <t>Nota mínima</t>
+  </si>
+  <si>
+    <t>Nota máxima</t>
   </si>
 </sst>
 </file>
@@ -165,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +205,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -214,11 +241,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -227,6 +280,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,13 +600,13 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -691,8 +754,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -758,20 +821,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -829,7 +894,7 @@
         <v>2.8</v>
       </c>
       <c r="I2" s="5">
-        <f>AVERAGE($F2:$H2)</f>
+        <f t="shared" ref="I2:I11" si="0">AVERAGE($F2:$H2)</f>
         <v>2.7666666666666671</v>
       </c>
     </row>
@@ -859,7 +924,7 @@
         <v>3.4</v>
       </c>
       <c r="I3" s="5">
-        <f>AVERAGE($F3:$H3)</f>
+        <f t="shared" si="0"/>
         <v>3.2666666666666671</v>
       </c>
     </row>
@@ -889,7 +954,7 @@
         <v>2.8</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" ref="I4:I11" si="0">AVERAGE($F4:$H4)</f>
+        <f t="shared" si="0"/>
         <v>3.3666666666666667</v>
       </c>
     </row>
@@ -1103,8 +1168,53 @@
         <v>3.1333333333333333</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="8">
+        <f>COUNTA(A2:A11)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="8">
+        <f>AVERAGE(I2:I11)</f>
+        <v>3.203333333333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="8">
+        <f>MIN(I2:I11)</f>
+        <v>2.7666666666666671</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="8">
+        <f>MAX(I2:I11)</f>
+        <v>3.6</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H11" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <mergeCells count="1">
+    <mergeCell ref="E13:F13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
   <headerFooter>

</xml_diff>

<commit_message>
codicional de excel rojo
</commit_message>
<xml_diff>
--- a/excel/16-ejecicio-excel-modificado.xlsx
+++ b/excel/16-ejecicio-excel-modificado.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JesusCarvajal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C695B7-DE76-4ACD-B045-C051270B934D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413877D0-F03B-4EA2-820F-BB37EAB72BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -233,19 +233,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -280,21 +267,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -600,7 +602,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -732,7 +734,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C11" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C11">
+      <sortCondition ref="A1:A11"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
   <headerFooter>
@@ -824,7 +830,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,7 +891,7 @@
         <v>23</v>
       </c>
       <c r="F2" s="2">
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
       <c r="G2" s="2">
         <v>3</v>
@@ -895,7 +901,7 @@
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I11" si="0">AVERAGE($F2:$H2)</f>
-        <v>2.7666666666666671</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1158,56 +1164,56 @@
         <v>3</v>
       </c>
       <c r="G11" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H11" s="2">
         <v>3.4</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="0"/>
-        <v>3.1333333333333333</v>
+        <v>3.8000000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <f>COUNTA(A2:A11)</f>
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="6">
         <f>AVERAGE(I2:I11)</f>
-        <v>3.203333333333334</v>
+        <v>3.2833333333333337</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="6">
         <f>MIN(I2:I11)</f>
-        <v>2.7666666666666671</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="6">
         <f>MAX(I2:I11)</f>
-        <v>3.6</v>
+        <v>3.8000000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1215,6 +1221,14 @@
   <mergeCells count="1">
     <mergeCell ref="E13:F13"/>
   </mergeCells>
+  <conditionalFormatting sqref="F2:I11">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
   <headerFooter>

</xml_diff>